<commit_message>
Update: Se actualiza Normalizacion excel
</commit_message>
<xml_diff>
--- a/2. Diseño/1. Normalización/Normalizacion.xlsx
+++ b/2. Diseño/1. Normalización/Normalizacion.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ADSI\PROYECTO\Base de datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\APRENDIZ\Documents\Git\tiendavirtual\2. Diseño\1. Normalización\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A870AC32-159F-47EA-B757-F7F32EC2E445}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12336"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -677,7 +678,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-240A]\ #,##0"/>
   </numFmts>
@@ -5430,8 +5431,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A5:G10" totalsRowShown="0" headerRowDxfId="191" dataDxfId="190">
-  <autoFilter ref="A5:G10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="A5:G10" totalsRowShown="0" headerRowDxfId="191" dataDxfId="190">
+  <autoFilter ref="A5:G10" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -5441,155 +5442,154 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" name="Id Usuario" dataDxfId="189"/>
-    <tableColumn id="2" name="Nombre  Usuario" dataDxfId="188"/>
-    <tableColumn id="3" name="Apellido Usuario" dataDxfId="187"/>
-    <tableColumn id="4" name="Correo  Usuario" dataDxfId="186" dataCellStyle="Hipervínculo"/>
-    <tableColumn id="5" name="Password" dataDxfId="185"/>
-    <tableColumn id="6" name="Ciudad" dataDxfId="184"/>
-    <tableColumn id="7" name="Dirección" dataDxfId="183"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id Usuario" dataDxfId="189"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Nombre  Usuario" dataDxfId="188"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Apellido Usuario" dataDxfId="187"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Correo  Usuario" dataDxfId="186" dataCellStyle="Hipervínculo"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Password" dataDxfId="185"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Ciudad" dataDxfId="184"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Dirección" dataDxfId="183"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="23" name="Tabla2224" displayName="Tabla2224" ref="AE14:AH19" totalsRowShown="0" headerRowDxfId="109" headerRowBorderDxfId="108" tableBorderDxfId="107" totalsRowBorderDxfId="106">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Tabla2224" displayName="Tabla2224" ref="AE14:AH19" totalsRowShown="0" headerRowDxfId="109" headerRowBorderDxfId="108" tableBorderDxfId="107" totalsRowBorderDxfId="106">
   <tableColumns count="4">
-    <tableColumn id="1" name="IdEnvios" dataDxfId="105"/>
-    <tableColumn id="2" name="Estado" dataDxfId="104"/>
-    <tableColumn id="3" name="Transportadora" dataDxfId="103"/>
-    <tableColumn id="4" name="CodigoRastreo" dataDxfId="102"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="IdEnvios" dataDxfId="105"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="Estado" dataDxfId="104"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="Transportadora" dataDxfId="103"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="CodigoRastreo" dataDxfId="102"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24" name="Tabla24" displayName="Tabla24" ref="AN5:AU10" totalsRowShown="0" headerRowDxfId="101" headerRowBorderDxfId="100" tableBorderDxfId="99" totalsRowBorderDxfId="98">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="Tabla24" displayName="Tabla24" ref="AN5:AU10" totalsRowShown="0" headerRowDxfId="101" headerRowBorderDxfId="100" tableBorderDxfId="99" totalsRowBorderDxfId="98">
   <tableColumns count="8">
-    <tableColumn id="1" name="IdProveedores" dataDxfId="97"/>
-    <tableColumn id="10" name="Contacto empresa" dataDxfId="96"/>
-    <tableColumn id="2" name="NombreEmpresa" dataDxfId="95"/>
-    <tableColumn id="9" name="Telefono y extensión" dataDxfId="94"/>
-    <tableColumn id="4" name="Direccion" dataDxfId="93"/>
-    <tableColumn id="5" name="WebSite" dataDxfId="92" dataCellStyle="Hipervínculo"/>
-    <tableColumn id="6" name="Email" dataDxfId="91" dataCellStyle="Hipervínculo"/>
-    <tableColumn id="7" name="RolEmpresa" dataDxfId="90"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="IdProveedores" dataDxfId="97"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0A00-00000A000000}" name="Contacto empresa" dataDxfId="96"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="NombreEmpresa" dataDxfId="95"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0A00-000009000000}" name="Telefono y extensión" dataDxfId="94"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0A00-000004000000}" name="Direccion" dataDxfId="93"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0A00-000005000000}" name="WebSite" dataDxfId="92" dataCellStyle="Hipervínculo"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0A00-000006000000}" name="Email" dataDxfId="91" dataCellStyle="Hipervínculo"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0A00-000007000000}" name="RolEmpresa" dataDxfId="90"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="25" name="Tabla2426" displayName="Tabla2426" ref="AI14:AR19" totalsRowShown="0" headerRowDxfId="89" headerRowBorderDxfId="88" tableBorderDxfId="87" totalsRowBorderDxfId="86">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="Tabla2426" displayName="Tabla2426" ref="AI14:AR19" totalsRowShown="0" headerRowDxfId="89" headerRowBorderDxfId="88" tableBorderDxfId="87" totalsRowBorderDxfId="86">
   <tableColumns count="10">
-    <tableColumn id="1" name="IdProveedores" dataDxfId="85"/>
-    <tableColumn id="2" name="NombreEmpresa" dataDxfId="84"/>
-    <tableColumn id="10" name="Nombre contacto empresa" dataDxfId="83"/>
-    <tableColumn id="3" name="Apellido contacto empresa" dataDxfId="82"/>
-    <tableColumn id="4" name="Telefono" dataDxfId="81"/>
-    <tableColumn id="9" name="Extension" dataDxfId="80"/>
-    <tableColumn id="5" name="Direccion" dataDxfId="79" dataCellStyle="Hipervínculo"/>
-    <tableColumn id="6" name="WebSite" dataDxfId="78" dataCellStyle="Hipervínculo"/>
-    <tableColumn id="7" name="Email" dataDxfId="77" dataCellStyle="Hipervínculo"/>
-    <tableColumn id="8" name="RolEmpresa" dataDxfId="76"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0B00-000001000000}" name="IdProveedores" dataDxfId="85"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name="NombreEmpresa" dataDxfId="84"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0B00-00000A000000}" name="Nombre contacto empresa" dataDxfId="83"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0B00-000003000000}" name="Apellido contacto empresa" dataDxfId="82"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0B00-000004000000}" name="Telefono" dataDxfId="81"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0B00-000009000000}" name="Extension" dataDxfId="80"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0B00-000005000000}" name="Direccion" dataDxfId="79" dataCellStyle="Hipervínculo"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0B00-000006000000}" name="WebSite" dataDxfId="78" dataCellStyle="Hipervínculo"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0B00-000007000000}" name="Email" dataDxfId="77" dataCellStyle="Hipervínculo"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0B00-000008000000}" name="RolEmpresa" dataDxfId="76"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Tabla21" displayName="Tabla21" ref="AA14:AD19" totalsRowShown="0" headerRowBorderDxfId="75" tableBorderDxfId="74" totalsRowBorderDxfId="73">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="Tabla21" displayName="Tabla21" ref="AA14:AD19" totalsRowShown="0" headerRowBorderDxfId="75" tableBorderDxfId="74" totalsRowBorderDxfId="73">
   <tableColumns count="4">
-    <tableColumn id="1" name="FechaDeVenta" dataDxfId="72"/>
-    <tableColumn id="2" name="Producto" dataDxfId="71"/>
-    <tableColumn id="3" name="IVA" dataDxfId="70"/>
-    <tableColumn id="4" name="Total" dataDxfId="69"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="FechaDeVenta" dataDxfId="72"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="Producto" dataDxfId="71"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0C00-000003000000}" name="IVA" dataDxfId="70"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0C00-000004000000}" name="Total" dataDxfId="69"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla16203" displayName="Tabla16203" ref="AB22:AE27" totalsRowShown="0" headerRowDxfId="68" dataDxfId="67" headerRowCellStyle="Normal" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF0D000000}" name="Tabla16203" displayName="Tabla16203" ref="AB22:AE27" totalsRowShown="0" headerRowDxfId="68" dataDxfId="67" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <tableColumns count="4">
-    <tableColumn id="1" name="IdGarantia" dataDxfId="66" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="EstadoGarantia" dataDxfId="65" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="FechaIngreso" dataDxfId="64" dataCellStyle="Normal"/>
-    <tableColumn id="4" name="Observaciones" dataDxfId="63" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0D00-000001000000}" name="IdGarantia" dataDxfId="66" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0D00-000002000000}" name="EstadoGarantia" dataDxfId="65" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0D00-000003000000}" name="FechaIngreso" dataDxfId="64" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0D00-000004000000}" name="Observaciones" dataDxfId="63" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla214" displayName="Tabla214" ref="X39:Y44" totalsRowShown="0" headerRowBorderDxfId="62" tableBorderDxfId="61" totalsRowBorderDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF0E000000}" name="Tabla214" displayName="Tabla214" ref="X39:Y44" totalsRowShown="0" headerRowBorderDxfId="62" tableBorderDxfId="61" totalsRowBorderDxfId="60">
   <tableColumns count="2">
-    <tableColumn id="1" name="FechaVenta" dataDxfId="59"/>
-    <tableColumn id="4" name="Total" dataDxfId="58"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0E00-000001000000}" name="FechaVenta" dataDxfId="59"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0E00-000004000000}" name="Total" dataDxfId="58"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla22245" displayName="Tabla22245" ref="AM22:AP27" totalsRowShown="0" headerRowDxfId="57" headerRowBorderDxfId="56" tableBorderDxfId="55" totalsRowBorderDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF0F000000}" name="Tabla22245" displayName="Tabla22245" ref="AM22:AP27" totalsRowShown="0" headerRowDxfId="57" headerRowBorderDxfId="56" tableBorderDxfId="55" totalsRowBorderDxfId="54">
   <tableColumns count="4">
-    <tableColumn id="1" name="IdEnvios" dataDxfId="53"/>
-    <tableColumn id="2" name="Estado" dataDxfId="52"/>
-    <tableColumn id="3" name="Transportadora" dataDxfId="51"/>
-    <tableColumn id="4" name="CodigoRastreo" dataDxfId="50"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0F00-000001000000}" name="IdEnvios" dataDxfId="53"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0F00-000002000000}" name="Estado" dataDxfId="52"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0F00-000003000000}" name="Transportadora" dataDxfId="51"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0F00-000004000000}" name="CodigoRastreo" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla10196" displayName="Tabla10196" ref="L22:P27" totalsRowShown="0" headerRowDxfId="49" dataDxfId="47" headerRowBorderDxfId="48" tableBorderDxfId="46" totalsRowBorderDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF10000000}" name="Tabla10196" displayName="Tabla10196" ref="L22:P27" totalsRowShown="0" headerRowDxfId="49" dataDxfId="47" headerRowBorderDxfId="48" tableBorderDxfId="46" totalsRowBorderDxfId="45">
   <tableColumns count="5">
-    <tableColumn id="1" name="IdCarritoCompras" dataDxfId="44"/>
-    <tableColumn id="2" name="Precio" dataDxfId="43"/>
-    <tableColumn id="3" name="NombreProducto" dataDxfId="42"/>
-    <tableColumn id="4" name="Imagen" dataDxfId="41"/>
-    <tableColumn id="6" name="Cantidad" dataDxfId="40"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1000-000001000000}" name="IdCarritoCompras" dataDxfId="44"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1000-000002000000}" name="Precio" dataDxfId="43"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1000-000003000000}" name="NombreProducto" dataDxfId="42"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1000-000004000000}" name="Imagen" dataDxfId="41"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1000-000006000000}" name="Cantidad" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla6" displayName="Tabla6" ref="R22:V27" totalsRowShown="0" headerRowBorderDxfId="39" tableBorderDxfId="38" totalsRowBorderDxfId="37">
-  <autoFilter ref="R22:V27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF11000000}" name="Tabla6" displayName="Tabla6" ref="R22:V27" totalsRowShown="0" headerRowBorderDxfId="39" tableBorderDxfId="38" totalsRowBorderDxfId="37">
+  <autoFilter ref="R22:V27" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="IdProductos" dataDxfId="36"/>
-    <tableColumn id="2" name="Nombre del producto" dataDxfId="35"/>
-    <tableColumn id="3" name="Descripcion2" dataDxfId="34"/>
-    <tableColumn id="4" name="existencias" dataDxfId="33"/>
-    <tableColumn id="5" name="Valor" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1100-000001000000}" name="IdProductos" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1100-000002000000}" name="Nombre del producto" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1100-000003000000}" name="Descripcion2" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1100-000004000000}" name="existencias" dataDxfId="33"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1100-000005000000}" name="Valor" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium24" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla68" displayName="Tabla68" ref="J39:O44" totalsRowShown="0" headerRowBorderDxfId="31" tableBorderDxfId="30" totalsRowBorderDxfId="29">
-  <autoFilter ref="J39:O44"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF12000000}" name="Tabla68" displayName="Tabla68" ref="J39:O44" totalsRowShown="0" headerRowBorderDxfId="31" tableBorderDxfId="30" totalsRowBorderDxfId="29">
   <tableColumns count="6">
-    <tableColumn id="1" name="IdProductos" dataDxfId="28"/>
-    <tableColumn id="2" name="Nombre del producto" dataDxfId="27"/>
-    <tableColumn id="3" name="Descripcion" dataDxfId="26"/>
-    <tableColumn id="4" name="existencias" dataDxfId="25"/>
-    <tableColumn id="6" name="imagen" dataDxfId="24"/>
-    <tableColumn id="5" name="Precio" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1200-000001000000}" name="IdProductos" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1200-000002000000}" name="Nombre del producto" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1200-000003000000}" name="Descripcion" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1200-000004000000}" name="existencias" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1200-000006000000}" name="imagen" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1200-000005000000}" name="Precio" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium24" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabla10" displayName="Tabla10" ref="H5:L10" totalsRowShown="0" headerRowDxfId="182" dataDxfId="180" headerRowBorderDxfId="181" tableBorderDxfId="179" totalsRowBorderDxfId="178">
-  <autoFilter ref="H5:L10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabla10" displayName="Tabla10" ref="H5:L10" totalsRowShown="0" headerRowDxfId="182" dataDxfId="180" headerRowBorderDxfId="181" tableBorderDxfId="179" totalsRowBorderDxfId="178">
+  <autoFilter ref="H5:L10" xr:uid="{00000000-0009-0000-0100-00000A000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -5597,62 +5597,62 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" name="IdCarritoCompras" dataDxfId="177"/>
-    <tableColumn id="2" name="Precio" dataDxfId="176"/>
-    <tableColumn id="3" name="NombreProducto" dataDxfId="175"/>
-    <tableColumn id="4" name="Imagen" dataDxfId="174"/>
-    <tableColumn id="5" name="Cantidad" dataDxfId="173"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="IdCarritoCompras" dataDxfId="177"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Precio" dataDxfId="176"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="NombreProducto" dataDxfId="175"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Imagen" dataDxfId="174"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Cantidad" dataDxfId="173"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabla162039" displayName="Tabla162039" ref="T39:U44" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" headerRowCellStyle="Normal" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF13000000}" name="Tabla162039" displayName="Tabla162039" ref="T39:U44" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <tableColumns count="2">
-    <tableColumn id="1" name="IdGarantia" dataDxfId="20" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="FechaIngreso" dataDxfId="19" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1300-000001000000}" name="IdGarantia" dataDxfId="20" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1300-000003000000}" name="FechaIngreso" dataDxfId="19" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tabla2113" displayName="Tabla2113" ref="AH22:AK27" totalsRowShown="0" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF14000000}" name="Tabla2113" displayName="Tabla2113" ref="AH22:AK27" totalsRowShown="0" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <tableColumns count="4">
-    <tableColumn id="1" name="FechaDeVenta" dataDxfId="15"/>
-    <tableColumn id="2" name="Producto" dataDxfId="14"/>
-    <tableColumn id="3" name="IVA" dataDxfId="13"/>
-    <tableColumn id="4" name="Total" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1400-000001000000}" name="FechaDeVenta" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1400-000002000000}" name="Producto" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1400-000003000000}" name="IVA" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1400-000004000000}" name="Total" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabla2224510" displayName="Tabla2224510" ref="AA39:AB44" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF15000000}" name="Tabla2224510" displayName="Tabla2224510" ref="AA39:AB44" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <tableColumns count="2">
-    <tableColumn id="1" name="IdEnvios" dataDxfId="7"/>
-    <tableColumn id="4" name="CodigoRastreo" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1500-000001000000}" name="IdEnvios" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1500-000004000000}" name="CodigoRastreo" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Tabla17" displayName="Tabla17" ref="W46:X58" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
-  <autoFilter ref="W46:X58"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF16000000}" name="Tabla17" displayName="Tabla17" ref="W46:X58" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
+  <autoFilter ref="W46:X58" xr:uid="{00000000-0009-0000-0100-000011000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="IdObservacion" dataDxfId="1"/>
-    <tableColumn id="2" name="Estado" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1600-000001000000}" name="IdObservacion" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1600-000002000000}" name="Estado" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tabla11" displayName="Tabla11" ref="M5:T12" totalsRowShown="0" headerRowDxfId="172" dataDxfId="170" headerRowBorderDxfId="171" tableBorderDxfId="169" totalsRowBorderDxfId="168">
-  <autoFilter ref="M5:T12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabla11" displayName="Tabla11" ref="M5:T12" totalsRowShown="0" headerRowDxfId="172" dataDxfId="170" headerRowBorderDxfId="171" tableBorderDxfId="169" totalsRowBorderDxfId="168">
+  <autoFilter ref="M5:T12" xr:uid="{00000000-0009-0000-0100-00000B000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -5663,89 +5663,89 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" name="IdProductos" dataDxfId="167"/>
-    <tableColumn id="2" name="Precio" dataDxfId="166"/>
-    <tableColumn id="3" name="Marca" dataDxfId="165"/>
-    <tableColumn id="4" name="Categoria" dataDxfId="164"/>
-    <tableColumn id="5" name="NombreProducto" dataDxfId="163"/>
-    <tableColumn id="6" name="Imagen" dataDxfId="162"/>
-    <tableColumn id="7" name="Descripcion" dataDxfId="161"/>
-    <tableColumn id="8" name="existencias" dataDxfId="160"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="IdProductos" dataDxfId="167"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Precio" dataDxfId="166"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Marca" dataDxfId="165"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Categoria" dataDxfId="164"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="NombreProducto" dataDxfId="163"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Imagen" dataDxfId="162"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Descripcion" dataDxfId="161"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="existencias" dataDxfId="160"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Tabla15" displayName="Tabla15" ref="U5:W10" totalsRowShown="0" headerRowDxfId="159" dataDxfId="157" headerRowBorderDxfId="158" tableBorderDxfId="156" totalsRowBorderDxfId="155">
-  <autoFilter ref="U5:W10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tabla15" displayName="Tabla15" ref="U5:W10" totalsRowShown="0" headerRowDxfId="159" dataDxfId="157" headerRowBorderDxfId="158" tableBorderDxfId="156" totalsRowBorderDxfId="155">
+  <autoFilter ref="U5:W10" xr:uid="{00000000-0009-0000-0100-00000F000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" name="IdCategoria" dataDxfId="154"/>
-    <tableColumn id="2" name="Marca" dataDxfId="153"/>
-    <tableColumn id="3" name="NombreCategoria" dataDxfId="152"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="IdCategoria" dataDxfId="154"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Marca" dataDxfId="153"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="NombreCategoria" dataDxfId="152"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Tabla16" displayName="Tabla16" ref="X5:AA10" totalsRowShown="0" headerRowDxfId="151" dataDxfId="150" headerRowCellStyle="Normal" dataCellStyle="Normal">
-  <autoFilter ref="X5:AA10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Tabla16" displayName="Tabla16" ref="X5:AA10" totalsRowShown="0" headerRowDxfId="151" dataDxfId="150" headerRowCellStyle="Normal" dataCellStyle="Normal">
+  <autoFilter ref="X5:AA10" xr:uid="{00000000-0009-0000-0100-000010000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" name="IdGarantia" dataDxfId="149" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="EstadoGarantia" dataDxfId="148" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="FechaIngreso" dataDxfId="147" dataCellStyle="Normal"/>
-    <tableColumn id="4" name="Observaciones" dataDxfId="146" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="IdGarantia" dataDxfId="149" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="EstadoGarantia" dataDxfId="148" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="FechaIngreso" dataDxfId="147" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Observaciones" dataDxfId="146" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Tabla1019" displayName="Tabla1019" ref="J14:N19" totalsRowShown="0" headerRowDxfId="145" dataDxfId="143" headerRowBorderDxfId="144" tableBorderDxfId="142" totalsRowBorderDxfId="141">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Tabla1019" displayName="Tabla1019" ref="J14:N19" totalsRowShown="0" headerRowDxfId="145" dataDxfId="143" headerRowBorderDxfId="144" tableBorderDxfId="142" totalsRowBorderDxfId="141">
   <tableColumns count="5">
-    <tableColumn id="1" name="IdCarritoCompras" dataDxfId="140"/>
-    <tableColumn id="2" name="Precio" dataDxfId="139"/>
-    <tableColumn id="3" name="NombreProducto" dataDxfId="138"/>
-    <tableColumn id="4" name="Imagen" dataDxfId="137"/>
-    <tableColumn id="5" name="Cantidad" dataDxfId="136"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="IdCarritoCompras" dataDxfId="140"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Precio" dataDxfId="139"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="NombreProducto" dataDxfId="138"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Imagen" dataDxfId="137"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Cantidad" dataDxfId="136"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Tabla1620" displayName="Tabla1620" ref="V14:Y19" totalsRowShown="0" headerRowDxfId="135" dataDxfId="134" headerRowCellStyle="Normal" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Tabla1620" displayName="Tabla1620" ref="V14:Y19" totalsRowShown="0" headerRowDxfId="135" dataDxfId="134" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <tableColumns count="4">
-    <tableColumn id="1" name="IdGarantia" dataDxfId="133" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="EstadoGarantia" dataDxfId="132" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="FechaIngreso" dataDxfId="131" dataCellStyle="Normal"/>
-    <tableColumn id="4" name="Observaciones" dataDxfId="130" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="IdGarantia" dataDxfId="133" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="EstadoGarantia" dataDxfId="132" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="FechaIngreso" dataDxfId="131" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="Observaciones" dataDxfId="130" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Tabla20" displayName="Tabla20" ref="AB5:AI10" totalsRowShown="0" headerRowDxfId="129" headerRowBorderDxfId="128" tableBorderDxfId="127" totalsRowBorderDxfId="126">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Tabla20" displayName="Tabla20" ref="AB5:AI10" totalsRowShown="0" headerRowDxfId="129" headerRowBorderDxfId="128" tableBorderDxfId="127" totalsRowBorderDxfId="126">
   <tableColumns count="8">
-    <tableColumn id="1" name="IdFacturacion" dataDxfId="125"/>
-    <tableColumn id="2" name="FechaDeVenta" dataDxfId="124"/>
-    <tableColumn id="3" name="Producto" dataDxfId="123"/>
-    <tableColumn id="4" name="Precio" dataDxfId="122"/>
-    <tableColumn id="5" name="Cantidad" dataDxfId="121"/>
-    <tableColumn id="6" name="IVA" dataDxfId="120"/>
-    <tableColumn id="7" name="NombreCliente" dataDxfId="119"/>
-    <tableColumn id="8" name="Total" dataDxfId="118">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="IdFacturacion" dataDxfId="125"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="FechaDeVenta" dataDxfId="124"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Producto" dataDxfId="123"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Precio" dataDxfId="122"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Cantidad" dataDxfId="121"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="IVA" dataDxfId="120"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="NombreCliente" dataDxfId="119"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0700-000008000000}" name="Total" dataDxfId="118">
       <calculatedColumnFormula>AE6*1.19</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5754,12 +5754,12 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="Tabla22" displayName="Tabla22" ref="AJ5:AM10" totalsRowShown="0" headerRowDxfId="117" headerRowBorderDxfId="116" tableBorderDxfId="115" totalsRowBorderDxfId="114">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Tabla22" displayName="Tabla22" ref="AJ5:AM10" totalsRowShown="0" headerRowDxfId="117" headerRowBorderDxfId="116" tableBorderDxfId="115" totalsRowBorderDxfId="114">
   <tableColumns count="4">
-    <tableColumn id="1" name="IdEnvios" dataDxfId="113"/>
-    <tableColumn id="2" name="Estado" dataDxfId="112"/>
-    <tableColumn id="3" name="Transportadora" dataDxfId="111"/>
-    <tableColumn id="4" name="CodigoRastreo" dataDxfId="110"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="IdEnvios" dataDxfId="113"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Estado" dataDxfId="112"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="Transportadora" dataDxfId="111"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="CodigoRastreo" dataDxfId="110"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6027,71 +6027,71 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AZ59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="T1" sqref="T1"/>
-      <selection pane="bottomLeft" activeCell="K46" sqref="K46"/>
+      <selection pane="bottomLeft" activeCell="K58" sqref="K58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.109375" style="35" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.88671875" style="36" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="29.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="66.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="29.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.21875" style="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" style="35" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="29.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="66.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" style="19" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9" style="19" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="66.5546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.88671875" style="19" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="66.5546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.6640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.5546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.88671875" style="19" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="24.33203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="66.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="66.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="24.28515625" style="19" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="48" style="19" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.44140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" style="19" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="48" style="19" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="29.21875" style="19" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.21875" style="19" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="29.21875" style="19" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="29.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="29.28515625" style="19" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="48" style="19" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.140625" style="19" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="14" style="19" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="13.6640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="29.21875" style="19" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="29.28515625" style="19" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="20" style="19" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="28" style="19" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="23.6640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="39" max="40" width="13.21875" style="19" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="16.44140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="23.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="39" max="40" width="13.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="16.42578125" style="19" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="20" style="19" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="28" style="19" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="16.109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="16.140625" style="19" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="20" style="19" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="28" style="19" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="23.6640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="8.44140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="9.109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="16.109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="23.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="8.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="9.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="16.140625" style="19" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="20" style="19" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="28" style="19" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="10.88671875" style="19" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="17.88671875" style="19" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="11.44140625" style="19"/>
-    <col min="56" max="56" width="22.44140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="32.88671875" style="19" bestFit="1" customWidth="1"/>
-    <col min="58" max="16384" width="11.44140625" style="19"/>
+    <col min="53" max="53" width="10.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="17.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="11.42578125" style="19"/>
+    <col min="56" max="56" width="22.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="32.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="58" max="16384" width="11.42578125" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:47" s="1" customFormat="1">
@@ -7085,7 +7085,7 @@
       <c r="U12" s="20"/>
       <c r="W12" s="22"/>
     </row>
-    <row r="13" spans="1:47" ht="31.2">
+    <row r="13" spans="1:47" ht="31.5">
       <c r="A13" s="114" t="s">
         <v>93</v>
       </c>
@@ -7944,7 +7944,7 @@
       <c r="U20" s="20"/>
       <c r="W20" s="22"/>
     </row>
-    <row r="21" spans="1:52" s="99" customFormat="1" ht="28.8">
+    <row r="21" spans="1:52" s="99" customFormat="1" ht="28.5">
       <c r="A21" s="96" t="s">
         <v>180</v>
       </c>
@@ -9048,7 +9048,7 @@
       <c r="F37" s="36"/>
       <c r="H37" s="19"/>
     </row>
-    <row r="38" spans="1:44" s="94" customFormat="1" ht="28.8">
+    <row r="38" spans="1:44" s="94" customFormat="1" ht="28.5">
       <c r="A38" s="93" t="s">
         <v>187</v>
       </c>
@@ -10040,66 +10040,66 @@
     <mergeCell ref="A4:AU4"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D6" r:id="rId1"/>
-    <hyperlink ref="D7" r:id="rId2"/>
-    <hyperlink ref="D8" r:id="rId3"/>
-    <hyperlink ref="D9" r:id="rId4"/>
-    <hyperlink ref="D10" r:id="rId5"/>
-    <hyperlink ref="AS6" r:id="rId6"/>
-    <hyperlink ref="AS7" r:id="rId7"/>
-    <hyperlink ref="AS8" r:id="rId8"/>
-    <hyperlink ref="AS9" r:id="rId9"/>
-    <hyperlink ref="AS10" r:id="rId10"/>
-    <hyperlink ref="AT6" r:id="rId11"/>
-    <hyperlink ref="AT7" r:id="rId12"/>
-    <hyperlink ref="AT8" r:id="rId13"/>
-    <hyperlink ref="AT9" r:id="rId14"/>
-    <hyperlink ref="AT10" r:id="rId15"/>
-    <hyperlink ref="F15" r:id="rId16"/>
-    <hyperlink ref="F16" r:id="rId17"/>
-    <hyperlink ref="F17" r:id="rId18"/>
-    <hyperlink ref="F18" r:id="rId19"/>
-    <hyperlink ref="F19" r:id="rId20"/>
-    <hyperlink ref="AP15" r:id="rId21"/>
-    <hyperlink ref="AP16" r:id="rId22"/>
-    <hyperlink ref="AP17" r:id="rId23"/>
-    <hyperlink ref="AP18" r:id="rId24"/>
-    <hyperlink ref="AP19" r:id="rId25"/>
-    <hyperlink ref="AQ15" r:id="rId26"/>
-    <hyperlink ref="AQ16" r:id="rId27"/>
-    <hyperlink ref="AQ17" r:id="rId28"/>
-    <hyperlink ref="AQ18" r:id="rId29"/>
-    <hyperlink ref="AQ19" r:id="rId30"/>
-    <hyperlink ref="F23" r:id="rId31"/>
-    <hyperlink ref="F24" r:id="rId32"/>
-    <hyperlink ref="F25" r:id="rId33"/>
-    <hyperlink ref="F26" r:id="rId34"/>
-    <hyperlink ref="F27" r:id="rId35"/>
-    <hyperlink ref="AY23" r:id="rId36"/>
-    <hyperlink ref="AY24" r:id="rId37"/>
-    <hyperlink ref="AY25" r:id="rId38"/>
-    <hyperlink ref="AY26" r:id="rId39"/>
-    <hyperlink ref="AY27" r:id="rId40"/>
-    <hyperlink ref="AZ23" r:id="rId41"/>
-    <hyperlink ref="AZ24" r:id="rId42"/>
-    <hyperlink ref="AZ25" r:id="rId43"/>
-    <hyperlink ref="AZ26" r:id="rId44"/>
-    <hyperlink ref="AZ27" r:id="rId45"/>
-    <hyperlink ref="F40" r:id="rId46"/>
-    <hyperlink ref="F41" r:id="rId47"/>
-    <hyperlink ref="F42" r:id="rId48"/>
-    <hyperlink ref="F43" r:id="rId49"/>
-    <hyperlink ref="F44" r:id="rId50"/>
-    <hyperlink ref="AJ40" r:id="rId51"/>
-    <hyperlink ref="AJ41" r:id="rId52"/>
-    <hyperlink ref="AJ42" r:id="rId53"/>
-    <hyperlink ref="AJ43" r:id="rId54"/>
-    <hyperlink ref="AJ44" r:id="rId55"/>
-    <hyperlink ref="AK40" r:id="rId56"/>
-    <hyperlink ref="AK41" r:id="rId57"/>
-    <hyperlink ref="AK42" r:id="rId58"/>
-    <hyperlink ref="AK43" r:id="rId59"/>
-    <hyperlink ref="AK44" r:id="rId60"/>
+    <hyperlink ref="D6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D7" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D8" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D9" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D10" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="AS6" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="AS7" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="AS8" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="AS9" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="AS10" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="AT6" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="AT7" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="AT8" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="AT9" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="AT10" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="F15" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="F16" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="F17" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="F18" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="F19" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="AP15" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="AP16" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="AP17" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="AP18" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="AP19" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="AQ15" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="AQ16" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="AQ17" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="AQ18" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="AQ19" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="F23" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="F24" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="F25" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="F26" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="F27" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="AY23" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="AY24" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="AY25" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="AY26" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="AY27" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="AZ23" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="AZ24" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="AZ25" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="AZ26" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="AZ27" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="F40" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="F41" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="F42" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="F43" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="F44" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="AJ40" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="AJ41" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="AJ42" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="AJ43" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="AJ44" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="AK40" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="AK41" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="AK42" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="AK43" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="AK44" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId61"/>

</xml_diff>